<commit_message>
Protests in Novokhopyorsk upd.
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/age extremums.xlsx
+++ b/migforecasting/clustering/age extremums.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="35">
   <si>
     <t>oktmo</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>город Курск</t>
+  </si>
+  <si>
+    <t>Новохопёрский муниципальный район</t>
   </si>
 </sst>
 </file>
@@ -453,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2089,6 +2092,118 @@
         <v>5.9630000000000002E-2</v>
       </c>
     </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>20627000</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2012</v>
+      </c>
+      <c r="E30" s="1">
+        <v>5.9569999999999998E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <v>5.3039999999999997E-2</v>
+      </c>
+      <c r="G30" s="1">
+        <v>5.57E-2</v>
+      </c>
+      <c r="H30" s="1">
+        <v>5.1450000000000003E-2</v>
+      </c>
+      <c r="I30" s="1">
+        <v>6.5369999999999998E-2</v>
+      </c>
+      <c r="J30" s="1">
+        <v>7.7899999999999997E-2</v>
+      </c>
+      <c r="K30" s="1">
+        <v>7.6899999999999996E-2</v>
+      </c>
+      <c r="L30" s="1">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="M30" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="N30" s="1">
+        <v>8.6099999999999996E-2</v>
+      </c>
+      <c r="O30" s="1">
+        <v>0.10284</v>
+      </c>
+      <c r="P30" s="1">
+        <v>8.9099999999999999E-2</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>8.5599999999999996E-2</v>
+      </c>
+      <c r="R30" s="1">
+        <v>4.4400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>20627000</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2012</v>
+      </c>
+      <c r="E31" s="1">
+        <v>6.1280000000000001E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <v>5.9360000000000003E-2</v>
+      </c>
+      <c r="G31" s="1">
+        <v>6.4899999999999999E-2</v>
+      </c>
+      <c r="H31" s="1">
+        <v>6.3600000000000004E-2</v>
+      </c>
+      <c r="I31" s="1">
+        <v>7.1400000000000005E-2</v>
+      </c>
+      <c r="J31" s="1">
+        <v>8.8599999999999998E-2</v>
+      </c>
+      <c r="K31" s="1">
+        <v>7.6700000000000004E-2</v>
+      </c>
+      <c r="L31" s="1">
+        <v>7.6300000000000007E-2</v>
+      </c>
+      <c r="M31" s="1">
+        <v>7.4300000000000005E-2</v>
+      </c>
+      <c r="N31" s="1">
+        <v>8.6300000000000002E-2</v>
+      </c>
+      <c r="O31" s="1">
+        <v>0.10297000000000001</v>
+      </c>
+      <c r="P31" s="1">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>6.6650000000000001E-2</v>
+      </c>
+      <c r="R31" s="1">
+        <v>2.6980000000000001E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
New local extreme (Kotlas)
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/age extremums.xlsx
+++ b/migforecasting/clustering/age extremums.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="36">
   <si>
     <t>oktmo</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Новохопёрский муниципальный район</t>
+  </si>
+  <si>
+    <t>город Котлас</t>
   </si>
 </sst>
 </file>
@@ -456,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R31"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2204,6 +2207,118 @@
         <v>2.6980000000000001E-2</v>
       </c>
     </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>11710000</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2019</v>
+      </c>
+      <c r="E32" s="1">
+        <v>5.8799999999999998E-2</v>
+      </c>
+      <c r="F32" s="1">
+        <v>6.7799999999999999E-2</v>
+      </c>
+      <c r="G32" s="1">
+        <v>6.0400000000000002E-2</v>
+      </c>
+      <c r="H32" s="1">
+        <v>4.6899999999999997E-2</v>
+      </c>
+      <c r="I32" s="1">
+        <v>3.168E-2</v>
+      </c>
+      <c r="J32" s="1">
+        <v>4.7940000000000003E-2</v>
+      </c>
+      <c r="K32" s="1">
+        <v>7.7149999999999996E-2</v>
+      </c>
+      <c r="L32" s="1">
+        <v>8.6550000000000002E-2</v>
+      </c>
+      <c r="M32" s="1">
+        <v>8.0259999999999998E-2</v>
+      </c>
+      <c r="N32" s="1">
+        <v>6.3049999999999995E-2</v>
+      </c>
+      <c r="O32" s="1">
+        <v>0.12759999999999999</v>
+      </c>
+      <c r="P32" s="1">
+        <v>8.0399999999999999E-2</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>9.3700000000000006E-2</v>
+      </c>
+      <c r="R32" s="1">
+        <v>7.7899999999999997E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>11710000</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2019</v>
+      </c>
+      <c r="E33" s="1">
+        <v>7.0430000000000006E-2</v>
+      </c>
+      <c r="F33" s="1">
+        <v>8.2150000000000001E-2</v>
+      </c>
+      <c r="G33" s="1">
+        <v>6.9760000000000003E-2</v>
+      </c>
+      <c r="H33" s="1">
+        <v>5.4100000000000002E-2</v>
+      </c>
+      <c r="I33" s="1">
+        <v>2.7189999999999999E-2</v>
+      </c>
+      <c r="J33" s="1">
+        <v>4.8550000000000003E-2</v>
+      </c>
+      <c r="K33" s="1">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="L33" s="1">
+        <v>0.10009999999999999</v>
+      </c>
+      <c r="M33" s="1">
+        <v>9.4539999999999999E-2</v>
+      </c>
+      <c r="N33" s="1">
+        <v>6.83E-2</v>
+      </c>
+      <c r="O33" s="1">
+        <v>0.11115</v>
+      </c>
+      <c r="P33" s="1">
+        <v>6.7500000000000004E-2</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>6.6500000000000004E-2</v>
+      </c>
+      <c r="R33" s="1">
+        <v>5.1670000000000001E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
new local extreme (Laishevsky)
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/age extremums.xlsx
+++ b/migforecasting/clustering/age extremums.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="37">
   <si>
     <t>oktmo</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>город Котлас</t>
+  </si>
+  <si>
+    <t>Лаишевский муниципальный район</t>
   </si>
 </sst>
 </file>
@@ -459,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2319,6 +2322,118 @@
         <v>5.1670000000000001E-2</v>
       </c>
     </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>92634000</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E34" s="1">
+        <v>6.1769999999999999E-2</v>
+      </c>
+      <c r="F34" s="1">
+        <v>6.7199999999999996E-2</v>
+      </c>
+      <c r="G34" s="1">
+        <v>5.21E-2</v>
+      </c>
+      <c r="H34" s="1">
+        <v>4.675E-2</v>
+      </c>
+      <c r="I34" s="1">
+        <v>4.8070000000000002E-2</v>
+      </c>
+      <c r="J34" s="1">
+        <v>7.0599999999999996E-2</v>
+      </c>
+      <c r="K34" s="1">
+        <v>9.35E-2</v>
+      </c>
+      <c r="L34" s="1">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="M34" s="1">
+        <v>6.7599999999999993E-2</v>
+      </c>
+      <c r="N34" s="1">
+        <v>5.9080000000000001E-2</v>
+      </c>
+      <c r="O34" s="1">
+        <v>0.12870000000000001</v>
+      </c>
+      <c r="P34" s="1">
+        <v>7.7759999999999996E-2</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>8.4659999999999999E-2</v>
+      </c>
+      <c r="R34" s="1">
+        <v>6.1519999999999998E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>92634000</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E35" s="1">
+        <v>6.7500000000000004E-2</v>
+      </c>
+      <c r="F35" s="1">
+        <v>7.6050000000000006E-2</v>
+      </c>
+      <c r="G35" s="1">
+        <v>5.7860000000000002E-2</v>
+      </c>
+      <c r="H35" s="1">
+        <v>4.8829999999999998E-2</v>
+      </c>
+      <c r="I35" s="1">
+        <v>4.376E-2</v>
+      </c>
+      <c r="J35" s="1">
+        <v>7.7299999999999994E-2</v>
+      </c>
+      <c r="K35" s="1">
+        <v>0.10564999999999999</v>
+      </c>
+      <c r="L35" s="1">
+        <v>8.0750000000000002E-2</v>
+      </c>
+      <c r="M35" s="1">
+        <v>7.22E-2</v>
+      </c>
+      <c r="N35" s="1">
+        <v>5.8779999999999999E-2</v>
+      </c>
+      <c r="O35" s="1">
+        <v>0.11940000000000001</v>
+      </c>
+      <c r="P35" s="1">
+        <v>7.0739999999999997E-2</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>7.2139999999999996E-2</v>
+      </c>
+      <c r="R35" s="1">
+        <v>4.9160000000000002E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
new local extremums (Gelendzhik & Anapa)
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/age extremums.xlsx
+++ b/migforecasting/clustering/age extremums.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="39">
   <si>
     <t>oktmo</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>Лаишевский муниципальный район</t>
+  </si>
+  <si>
+    <t>город-курорт Анапа</t>
+  </si>
+  <si>
+    <t>город-курорт Геленджик</t>
   </si>
 </sst>
 </file>
@@ -462,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R35"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2434,6 +2440,230 @@
         <v>4.9160000000000002E-2</v>
       </c>
     </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>3703000</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="1">
+        <v>2021</v>
+      </c>
+      <c r="E36" s="1">
+        <v>6.0760000000000002E-2</v>
+      </c>
+      <c r="F36" s="1">
+        <v>6.207E-2</v>
+      </c>
+      <c r="G36" s="1">
+        <v>5.2670000000000002E-2</v>
+      </c>
+      <c r="H36" s="1">
+        <v>4.6539999999999998E-2</v>
+      </c>
+      <c r="I36" s="1">
+        <v>3.8420000000000003E-2</v>
+      </c>
+      <c r="J36" s="1">
+        <v>5.6599999999999998E-2</v>
+      </c>
+      <c r="K36" s="1">
+        <v>8.0299999999999996E-2</v>
+      </c>
+      <c r="L36" s="1">
+        <v>8.8440000000000005E-2</v>
+      </c>
+      <c r="M36" s="1">
+        <v>7.8899999999999998E-2</v>
+      </c>
+      <c r="N36" s="1">
+        <v>7.0499999999999993E-2</v>
+      </c>
+      <c r="O36" s="1">
+        <v>0.1244</v>
+      </c>
+      <c r="P36" s="1">
+        <v>7.6050000000000006E-2</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>8.7599999999999997E-2</v>
+      </c>
+      <c r="R36" s="1">
+        <v>7.6799999999999993E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>3703000</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="1">
+        <v>2021</v>
+      </c>
+      <c r="E37" s="1">
+        <v>7.1840000000000001E-2</v>
+      </c>
+      <c r="F37" s="1">
+        <v>7.4300000000000005E-2</v>
+      </c>
+      <c r="G37" s="1">
+        <v>6.4699999999999994E-2</v>
+      </c>
+      <c r="H37" s="1">
+        <v>5.2600000000000001E-2</v>
+      </c>
+      <c r="I37" s="1">
+        <v>4.1320000000000003E-2</v>
+      </c>
+      <c r="J37" s="1">
+        <v>6.93E-2</v>
+      </c>
+      <c r="K37" s="1">
+        <v>8.9539999999999995E-2</v>
+      </c>
+      <c r="L37" s="1">
+        <v>8.4099999999999994E-2</v>
+      </c>
+      <c r="M37" s="1">
+        <v>7.6539999999999997E-2</v>
+      </c>
+      <c r="N37" s="1">
+        <v>6.9800000000000001E-2</v>
+      </c>
+      <c r="O37" s="1">
+        <v>0.11053</v>
+      </c>
+      <c r="P37" s="1">
+        <v>6.5100000000000005E-2</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>7.0400000000000004E-2</v>
+      </c>
+      <c r="R37" s="1">
+        <v>5.9970000000000002E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>3708000</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="1">
+        <v>2021</v>
+      </c>
+      <c r="E38" s="1">
+        <v>5.774E-2</v>
+      </c>
+      <c r="F38" s="1">
+        <v>6.0199999999999997E-2</v>
+      </c>
+      <c r="G38" s="1">
+        <v>5.1479999999999998E-2</v>
+      </c>
+      <c r="H38" s="1">
+        <v>4.2569999999999997E-2</v>
+      </c>
+      <c r="I38" s="1">
+        <v>3.5430000000000003E-2</v>
+      </c>
+      <c r="J38" s="1">
+        <v>4.437E-2</v>
+      </c>
+      <c r="K38" s="1">
+        <v>8.0140000000000003E-2</v>
+      </c>
+      <c r="L38" s="1">
+        <v>9.2499999999999999E-2</v>
+      </c>
+      <c r="M38" s="1">
+        <v>8.3599999999999994E-2</v>
+      </c>
+      <c r="N38" s="1">
+        <v>7.4700000000000003E-2</v>
+      </c>
+      <c r="O38" s="1">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="P38" s="1">
+        <v>7.8299999999999995E-2</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>8.8900000000000007E-2</v>
+      </c>
+      <c r="R38" s="1">
+        <v>7.9039999999999999E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>3708000</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="1">
+        <v>2021</v>
+      </c>
+      <c r="E39" s="1">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="F39" s="1">
+        <v>7.2749999999999995E-2</v>
+      </c>
+      <c r="G39" s="1">
+        <v>6.1830000000000003E-2</v>
+      </c>
+      <c r="H39" s="1">
+        <v>5.0659999999999997E-2</v>
+      </c>
+      <c r="I39" s="1">
+        <v>4.0399999999999998E-2</v>
+      </c>
+      <c r="J39" s="1">
+        <v>5.3220000000000003E-2</v>
+      </c>
+      <c r="K39" s="1">
+        <v>8.0750000000000002E-2</v>
+      </c>
+      <c r="L39" s="1">
+        <v>9.1740000000000002E-2</v>
+      </c>
+      <c r="M39" s="1">
+        <v>8.5629999999999998E-2</v>
+      </c>
+      <c r="N39" s="1">
+        <v>7.1349999999999997E-2</v>
+      </c>
+      <c r="O39" s="1">
+        <v>0.11890000000000001</v>
+      </c>
+      <c r="P39" s="1">
+        <v>6.8900000000000003E-2</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="R39" s="1">
+        <v>6.2799999999999995E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
New local extremum (Angarsk)
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/age extremums.xlsx
+++ b/migforecasting/clustering/age extremums.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="40">
   <si>
     <t>oktmo</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>город-курорт Геленджик</t>
+  </si>
+  <si>
+    <t>Ангарский</t>
   </si>
 </sst>
 </file>
@@ -468,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R39"/>
+  <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="T31" sqref="T31"/>
+      <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2664,6 +2667,118 @@
         <v>6.2799999999999995E-2</v>
       </c>
     </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>25703000</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E40" s="1">
+        <v>5.8500000000000003E-2</v>
+      </c>
+      <c r="F40" s="1">
+        <v>6.5729999999999997E-2</v>
+      </c>
+      <c r="G40" s="1">
+        <v>5.5899999999999998E-2</v>
+      </c>
+      <c r="H40" s="1">
+        <v>4.904E-2</v>
+      </c>
+      <c r="I40" s="1">
+        <v>4.4220000000000002E-2</v>
+      </c>
+      <c r="J40" s="1">
+        <v>6.0639999999999999E-2</v>
+      </c>
+      <c r="K40" s="1">
+        <v>8.6900000000000005E-2</v>
+      </c>
+      <c r="L40" s="1">
+        <v>8.48E-2</v>
+      </c>
+      <c r="M40" s="1">
+        <v>7.6350000000000001E-2</v>
+      </c>
+      <c r="N40" s="1">
+        <v>7.2900000000000006E-2</v>
+      </c>
+      <c r="O40" s="1">
+        <v>0.12256</v>
+      </c>
+      <c r="P40" s="1">
+        <v>7.3200000000000001E-2</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>7.7799999999999994E-2</v>
+      </c>
+      <c r="R40" s="1">
+        <v>7.1529999999999996E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>25703000</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E41" s="1">
+        <v>6.7599999999999993E-2</v>
+      </c>
+      <c r="F41" s="1">
+        <v>7.3499999999999996E-2</v>
+      </c>
+      <c r="G41" s="1">
+        <v>6.3700000000000007E-2</v>
+      </c>
+      <c r="H41" s="1">
+        <v>5.7619999999999998E-2</v>
+      </c>
+      <c r="I41" s="1">
+        <v>5.28E-2</v>
+      </c>
+      <c r="J41" s="1">
+        <v>7.2139999999999996E-2</v>
+      </c>
+      <c r="K41" s="1">
+        <v>0.10266</v>
+      </c>
+      <c r="L41" s="1">
+        <v>9.6299999999999997E-2</v>
+      </c>
+      <c r="M41" s="1">
+        <v>7.8060000000000004E-2</v>
+      </c>
+      <c r="N41" s="1">
+        <v>7.1599999999999997E-2</v>
+      </c>
+      <c r="O41" s="1">
+        <v>0.10639999999999999</v>
+      </c>
+      <c r="P41" s="1">
+        <v>6.0850000000000001E-2</v>
+      </c>
+      <c r="Q41" s="1">
+        <v>5.3499999999999999E-2</v>
+      </c>
+      <c r="R41" s="1">
+        <v>4.3099999999999999E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
New local extremum (Altai)
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/age extremums.xlsx
+++ b/migforecasting/clustering/age extremums.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="41">
   <si>
     <t>oktmo</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Ангарский</t>
+  </si>
+  <si>
+    <t>Чойский муниципальный район</t>
   </si>
 </sst>
 </file>
@@ -471,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R41"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="S32" sqref="S32"/>
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2779,6 +2782,118 @@
         <v>4.3099999999999999E-2</v>
       </c>
     </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>84645000</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E42" s="1">
+        <v>7.1499999999999994E-2</v>
+      </c>
+      <c r="F42" s="1">
+        <v>9.2469999999999997E-2</v>
+      </c>
+      <c r="G42" s="1">
+        <v>7.6799999999999993E-2</v>
+      </c>
+      <c r="H42" s="1">
+        <v>4.8770000000000001E-2</v>
+      </c>
+      <c r="I42" s="1">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="J42" s="1">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="K42" s="1">
+        <v>8.5500000000000007E-2</v>
+      </c>
+      <c r="L42" s="1">
+        <v>6.8849999999999995E-2</v>
+      </c>
+      <c r="M42" s="1">
+        <v>7.3899999999999993E-2</v>
+      </c>
+      <c r="N42" s="1">
+        <v>6.54E-2</v>
+      </c>
+      <c r="O42" s="1">
+        <v>0.14050000000000001</v>
+      </c>
+      <c r="P42" s="1">
+        <v>7.9469999999999999E-2</v>
+      </c>
+      <c r="Q42" s="1">
+        <v>7.51E-2</v>
+      </c>
+      <c r="R42" s="1">
+        <v>4.7100000000000003E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>84645000</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E43" s="1">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="F43" s="1">
+        <v>9.4500000000000001E-2</v>
+      </c>
+      <c r="G43" s="1">
+        <v>7.6350000000000001E-2</v>
+      </c>
+      <c r="H43" s="1">
+        <v>6.216E-2</v>
+      </c>
+      <c r="I43" s="1">
+        <v>4.7500000000000001E-2</v>
+      </c>
+      <c r="J43" s="1">
+        <v>4.0280000000000003E-2</v>
+      </c>
+      <c r="K43" s="1">
+        <v>7.5200000000000003E-2</v>
+      </c>
+      <c r="L43" s="1">
+        <v>7.8899999999999998E-2</v>
+      </c>
+      <c r="M43" s="1">
+        <v>7.263E-2</v>
+      </c>
+      <c r="N43" s="1">
+        <v>5.5399999999999998E-2</v>
+      </c>
+      <c r="O43" s="1">
+        <v>0.12759999999999999</v>
+      </c>
+      <c r="P43" s="1">
+        <v>7.8700000000000006E-2</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>7.1499999999999994E-2</v>
+      </c>
+      <c r="R43" s="1">
+        <v>4.19E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
upd. order of the extremums
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/age extremums.xlsx
+++ b/migforecasting/clustering/age extremums.xlsx
@@ -476,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,898 +880,898 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>56613000</v>
+        <v>1630000</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="1">
-        <v>2019</v>
+        <v>2023</v>
       </c>
       <c r="E8" s="1">
-        <v>5.5329999999999997E-2</v>
+        <v>4.2720000000000001E-2</v>
       </c>
       <c r="F8" s="1">
-        <v>5.8099999999999999E-2</v>
+        <v>6.8849999999999995E-2</v>
       </c>
       <c r="G8" s="1">
-        <v>5.4960000000000002E-2</v>
+        <v>7.22E-2</v>
       </c>
       <c r="H8" s="1">
-        <v>4.3099999999999999E-2</v>
+        <v>6.3899999999999998E-2</v>
       </c>
       <c r="I8" s="1">
-        <v>4.0250000000000001E-2</v>
+        <v>4.1750000000000002E-2</v>
       </c>
       <c r="J8" s="1">
-        <v>5.5660000000000001E-2</v>
+        <v>3.424E-2</v>
       </c>
       <c r="K8" s="1">
-        <v>8.2500000000000004E-2</v>
+        <v>4.9770000000000002E-2</v>
       </c>
       <c r="L8" s="1">
-        <v>7.7200000000000005E-2</v>
+        <v>8.0699999999999994E-2</v>
       </c>
       <c r="M8" s="1">
-        <v>7.0739999999999997E-2</v>
+        <v>8.2150000000000001E-2</v>
       </c>
       <c r="N8" s="1">
-        <v>6.4449999999999993E-2</v>
+        <v>7.5800000000000006E-2</v>
       </c>
       <c r="O8" s="1">
-        <v>0.14199999999999999</v>
+        <v>0.12085</v>
       </c>
       <c r="P8" s="1">
-        <v>8.8200000000000001E-2</v>
+        <v>6.726E-2</v>
       </c>
       <c r="Q8" s="1">
-        <v>9.1899999999999996E-2</v>
+        <v>0.1027</v>
       </c>
       <c r="R8" s="1">
-        <v>7.5560000000000002E-2</v>
+        <v>9.7100000000000006E-2</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>56613000</v>
+        <v>1630000</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="1">
-        <v>2019</v>
+        <v>2023</v>
       </c>
       <c r="E9" s="1">
-        <v>6.1199999999999997E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F9" s="1">
-        <v>6.7299999999999999E-2</v>
+        <v>7.5700000000000003E-2</v>
       </c>
       <c r="G9" s="1">
-        <v>5.91E-2</v>
+        <v>8.2799999999999999E-2</v>
       </c>
       <c r="H9" s="1">
-        <v>4.938E-2</v>
+        <v>7.6300000000000007E-2</v>
       </c>
       <c r="I9" s="1">
-        <v>4.2500000000000003E-2</v>
+        <v>5.6149999999999999E-2</v>
       </c>
       <c r="J9" s="1">
-        <v>6.0729999999999999E-2</v>
+        <v>4.5260000000000002E-2</v>
       </c>
       <c r="K9" s="1">
-        <v>9.0149999999999994E-2</v>
+        <v>5.8069999999999997E-2</v>
       </c>
       <c r="L9" s="1">
-        <v>8.5099999999999995E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="M9" s="1">
-        <v>7.5600000000000001E-2</v>
+        <v>7.8899999999999998E-2</v>
       </c>
       <c r="N9" s="1">
-        <v>6.5799999999999997E-2</v>
+        <v>7.4800000000000005E-2</v>
       </c>
       <c r="O9" s="1">
-        <v>0.12989999999999999</v>
+        <v>0.1106</v>
       </c>
       <c r="P9" s="1">
-        <v>8.1900000000000001E-2</v>
+        <v>6.2469999999999998E-2</v>
       </c>
       <c r="Q9" s="1">
-        <v>7.4160000000000004E-2</v>
+        <v>8.4199999999999997E-2</v>
       </c>
       <c r="R9" s="1">
-        <v>5.7099999999999998E-2</v>
+        <v>6.7699999999999996E-2</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>63637000</v>
+        <v>33618000</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="1">
-        <v>2013</v>
+        <v>2020</v>
       </c>
       <c r="E10" s="1">
-        <v>6.1199999999999997E-2</v>
+        <v>4.514E-2</v>
       </c>
       <c r="F10" s="1">
-        <v>5.79E-2</v>
+        <v>6.9339999999999999E-2</v>
       </c>
       <c r="G10" s="1">
-        <v>5.1180000000000003E-2</v>
+        <v>5.6640000000000003E-2</v>
       </c>
       <c r="H10" s="1">
-        <v>5.246E-2</v>
+        <v>3.7350000000000001E-2</v>
       </c>
       <c r="I10" s="1">
-        <v>5.9229999999999998E-2</v>
+        <v>4.5319999999999999E-2</v>
       </c>
       <c r="J10" s="1">
-        <v>7.6300000000000007E-2</v>
+        <v>2.5250000000000002E-2</v>
       </c>
       <c r="K10" s="1">
-        <v>7.4770000000000003E-2</v>
+        <v>5.8169999999999999E-2</v>
       </c>
       <c r="L10" s="1">
-        <v>7.1499999999999994E-2</v>
+        <v>6.7900000000000002E-2</v>
       </c>
       <c r="M10" s="1">
-        <v>6.6799999999999998E-2</v>
+        <v>6.3E-2</v>
       </c>
       <c r="N10" s="1">
-        <v>7.4499999999999997E-2</v>
+        <v>6.3839999999999994E-2</v>
       </c>
       <c r="O10" s="1">
-        <v>0.16220000000000001</v>
+        <v>0.15229999999999999</v>
       </c>
       <c r="P10" s="1">
-        <v>8.6599999999999996E-2</v>
+        <v>0.10034</v>
       </c>
       <c r="Q10" s="1">
-        <v>6.6830000000000001E-2</v>
+        <v>0.12164</v>
       </c>
       <c r="R10" s="1">
-        <v>3.85E-2</v>
+        <v>9.3799999999999994E-2</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>63637000</v>
+        <v>33618000</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="1">
-        <v>2013</v>
+        <v>2020</v>
       </c>
       <c r="E11" s="1">
-        <v>5.79E-2</v>
+        <v>5.1479999999999998E-2</v>
       </c>
       <c r="F11" s="1">
-        <v>5.5629999999999999E-2</v>
+        <v>7.7499999999999999E-2</v>
       </c>
       <c r="G11" s="1">
-        <v>5.1639999999999998E-2</v>
+        <v>5.9900000000000002E-2</v>
       </c>
       <c r="H11" s="1">
-        <v>5.2519999999999997E-2</v>
+        <v>4.0340000000000001E-2</v>
       </c>
       <c r="I11" s="1">
-        <v>5.8930000000000003E-2</v>
+        <v>4.2880000000000001E-2</v>
       </c>
       <c r="J11" s="1">
-        <v>9.2700000000000005E-2</v>
+        <v>5.0840000000000003E-2</v>
       </c>
       <c r="K11" s="1">
-        <v>9.2100000000000001E-2</v>
+        <v>8.5750000000000007E-2</v>
       </c>
       <c r="L11" s="1">
-        <v>8.1600000000000006E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="M11" s="1">
-        <v>7.4899999999999994E-2</v>
+        <v>6.9339999999999999E-2</v>
       </c>
       <c r="N11" s="1">
-        <v>7.46E-2</v>
+        <v>6.2899999999999998E-2</v>
       </c>
       <c r="O11" s="1">
-        <v>0.14929999999999999</v>
+        <v>0.1323</v>
       </c>
       <c r="P11" s="1">
-        <v>7.886E-2</v>
+        <v>8.48E-2</v>
       </c>
       <c r="Q11" s="1">
-        <v>5.466E-2</v>
+        <v>8.9399999999999993E-2</v>
       </c>
       <c r="R11" s="1">
-        <v>2.4639999999999999E-2</v>
+        <v>6.8540000000000004E-2</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>75633000</v>
+        <v>11710000</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="1">
-        <v>2023</v>
+        <v>2019</v>
       </c>
       <c r="E12" s="1">
-        <v>0.05</v>
+        <v>5.8799999999999998E-2</v>
       </c>
       <c r="F12" s="1">
-        <v>7.5740000000000002E-2</v>
+        <v>6.7799999999999999E-2</v>
       </c>
       <c r="G12" s="1">
-        <v>7.3550000000000004E-2</v>
+        <v>6.0400000000000002E-2</v>
       </c>
       <c r="H12" s="1">
-        <v>5.6270000000000001E-2</v>
+        <v>4.6899999999999997E-2</v>
       </c>
       <c r="I12" s="1">
-        <v>4.5870000000000001E-2</v>
+        <v>3.168E-2</v>
       </c>
       <c r="J12" s="1">
-        <v>4.0370000000000003E-2</v>
+        <v>4.7940000000000003E-2</v>
       </c>
       <c r="K12" s="1">
-        <v>6.3350000000000004E-2</v>
+        <v>7.7149999999999996E-2</v>
       </c>
       <c r="L12" s="1">
-        <v>8.2400000000000001E-2</v>
+        <v>8.6550000000000002E-2</v>
       </c>
       <c r="M12" s="1">
-        <v>8.3000000000000004E-2</v>
+        <v>8.0259999999999998E-2</v>
       </c>
       <c r="N12" s="1">
-        <v>7.7499999999999999E-2</v>
+        <v>6.3049999999999995E-2</v>
       </c>
       <c r="O12" s="1">
-        <v>0.11285000000000001</v>
+        <v>0.12759999999999999</v>
       </c>
       <c r="P12" s="1">
-        <v>6.2560000000000004E-2</v>
+        <v>8.0399999999999999E-2</v>
       </c>
       <c r="Q12" s="1">
-        <v>9.1399999999999995E-2</v>
+        <v>9.3700000000000006E-2</v>
       </c>
       <c r="R12" s="1">
-        <v>8.5199999999999998E-2</v>
+        <v>7.7899999999999997E-2</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>75633000</v>
+        <v>11710000</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="1">
-        <v>2023</v>
+        <v>2019</v>
       </c>
       <c r="E13" s="1">
-        <v>6.25E-2</v>
+        <v>7.0430000000000006E-2</v>
       </c>
       <c r="F13" s="1">
-        <v>9.3799999999999994E-2</v>
+        <v>8.2150000000000001E-2</v>
       </c>
       <c r="G13" s="1">
-        <v>9.1800000000000007E-2</v>
+        <v>6.9760000000000003E-2</v>
       </c>
       <c r="H13" s="1">
-        <v>6.0299999999999999E-2</v>
+        <v>5.4100000000000002E-2</v>
       </c>
       <c r="I13" s="1">
-        <v>2.7019999999999999E-2</v>
+        <v>2.7189999999999999E-2</v>
       </c>
       <c r="J13" s="1">
-        <v>3.8100000000000002E-2</v>
+        <v>4.8550000000000003E-2</v>
       </c>
       <c r="K13" s="1">
-        <v>8.1799999999999998E-2</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="L13" s="1">
-        <v>9.0639999999999998E-2</v>
+        <v>0.10009999999999999</v>
       </c>
       <c r="M13" s="1">
-        <v>7.4899999999999994E-2</v>
+        <v>9.4539999999999999E-2</v>
       </c>
       <c r="N13" s="1">
-        <v>7.3700000000000002E-2</v>
+        <v>6.83E-2</v>
       </c>
       <c r="O13" s="1">
-        <v>0.1051</v>
+        <v>0.11115</v>
       </c>
       <c r="P13" s="1">
-        <v>5.6730000000000003E-2</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="Q13" s="1">
-        <v>7.5999999999999998E-2</v>
+        <v>6.6500000000000004E-2</v>
       </c>
       <c r="R13" s="1">
-        <v>6.7599999999999993E-2</v>
+        <v>5.1670000000000001E-2</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>80631000</v>
+        <v>56613000</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E14" s="1">
-        <v>5.713E-2</v>
+        <v>5.5329999999999997E-2</v>
       </c>
       <c r="F14" s="1">
-        <v>6.6350000000000006E-2</v>
+        <v>5.8099999999999999E-2</v>
       </c>
       <c r="G14" s="1">
-        <v>6.54E-2</v>
+        <v>5.4960000000000002E-2</v>
       </c>
       <c r="H14" s="1">
-        <v>4.7969999999999999E-2</v>
+        <v>4.3099999999999999E-2</v>
       </c>
       <c r="I14" s="1">
-        <v>4.8160000000000001E-2</v>
+        <v>4.0250000000000001E-2</v>
       </c>
       <c r="J14" s="1">
-        <v>4.5749999999999999E-2</v>
+        <v>5.5660000000000001E-2</v>
       </c>
       <c r="K14" s="1">
-        <v>7.306E-2</v>
+        <v>8.2500000000000004E-2</v>
       </c>
       <c r="L14" s="1">
-        <v>7.0499999999999993E-2</v>
+        <v>7.7200000000000005E-2</v>
       </c>
       <c r="M14" s="1">
-        <v>6.5699999999999995E-2</v>
+        <v>7.0739999999999997E-2</v>
       </c>
       <c r="N14" s="1">
-        <v>6.1429999999999998E-2</v>
+        <v>6.4449999999999993E-2</v>
       </c>
       <c r="O14" s="1">
-        <v>0.14660000000000001</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="P14" s="1">
-        <v>9.0639999999999998E-2</v>
+        <v>8.8200000000000001E-2</v>
       </c>
       <c r="Q14" s="1">
-        <v>8.7499999999999994E-2</v>
+        <v>9.1899999999999996E-2</v>
       </c>
       <c r="R14" s="1">
-        <v>7.3700000000000002E-2</v>
+        <v>7.5560000000000002E-2</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>80631000</v>
+        <v>56613000</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E15" s="1">
-        <v>6.1899999999999997E-2</v>
+        <v>6.1199999999999997E-2</v>
       </c>
       <c r="F15" s="1">
-        <v>7.1800000000000003E-2</v>
+        <v>6.7299999999999999E-2</v>
       </c>
       <c r="G15" s="1">
-        <v>6.9099999999999995E-2</v>
+        <v>5.91E-2</v>
       </c>
       <c r="H15" s="1">
-        <v>5.1240000000000001E-2</v>
+        <v>4.938E-2</v>
       </c>
       <c r="I15" s="1">
-        <v>4.446E-2</v>
+        <v>4.2500000000000003E-2</v>
       </c>
       <c r="J15" s="1">
-        <v>8.0439999999999998E-2</v>
+        <v>6.0729999999999999E-2</v>
       </c>
       <c r="K15" s="1">
-        <v>9.3899999999999997E-2</v>
+        <v>9.0149999999999994E-2</v>
       </c>
       <c r="L15" s="1">
-        <v>7.5130000000000002E-2</v>
+        <v>8.5099999999999995E-2</v>
       </c>
       <c r="M15" s="1">
-        <v>6.3600000000000004E-2</v>
+        <v>7.5600000000000001E-2</v>
       </c>
       <c r="N15" s="1">
-        <v>6.1039999999999997E-2</v>
+        <v>6.5799999999999997E-2</v>
       </c>
       <c r="O15" s="1">
-        <v>0.1278</v>
+        <v>0.12989999999999999</v>
       </c>
       <c r="P15" s="1">
-        <v>7.6969999999999997E-2</v>
+        <v>8.1900000000000001E-2</v>
       </c>
       <c r="Q15" s="1">
-        <v>7.2900000000000006E-2</v>
+        <v>7.4160000000000004E-2</v>
       </c>
       <c r="R15" s="1">
-        <v>4.9840000000000002E-2</v>
+        <v>5.7099999999999998E-2</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>80601000</v>
+        <v>63637000</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="1">
-        <v>2020</v>
+        <v>2013</v>
       </c>
       <c r="E16" s="1">
-        <v>7.2270000000000001E-2</v>
+        <v>6.1199999999999997E-2</v>
       </c>
       <c r="F16" s="1">
-        <v>8.7160000000000001E-2</v>
+        <v>5.79E-2</v>
       </c>
       <c r="G16" s="1">
-        <v>8.0140000000000003E-2</v>
+        <v>5.1180000000000003E-2</v>
       </c>
       <c r="H16" s="1">
-        <v>5.5300000000000002E-2</v>
+        <v>5.246E-2</v>
       </c>
       <c r="I16" s="1">
-        <v>5.79E-2</v>
+        <v>5.9229999999999998E-2</v>
       </c>
       <c r="J16" s="1">
-        <v>4.1930000000000002E-2</v>
+        <v>7.6300000000000007E-2</v>
       </c>
       <c r="K16" s="1">
-        <v>6.9599999999999995E-2</v>
+        <v>7.4770000000000003E-2</v>
       </c>
       <c r="L16" s="1">
-        <v>6.2469999999999998E-2</v>
+        <v>7.1499999999999994E-2</v>
       </c>
       <c r="M16" s="1">
-        <v>6.2560000000000004E-2</v>
+        <v>6.6799999999999998E-2</v>
       </c>
       <c r="N16" s="1">
-        <v>5.91E-2</v>
+        <v>7.4499999999999997E-2</v>
       </c>
       <c r="O16" s="1">
-        <v>0.14610000000000001</v>
+        <v>0.16220000000000001</v>
       </c>
       <c r="P16" s="1">
-        <v>8.5139999999999993E-2</v>
+        <v>8.6599999999999996E-2</v>
       </c>
       <c r="Q16" s="1">
-        <v>7.1900000000000006E-2</v>
+        <v>6.6830000000000001E-2</v>
       </c>
       <c r="R16" s="1">
-        <v>4.8500000000000001E-2</v>
+        <v>3.85E-2</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>80601000</v>
+        <v>63637000</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="1">
-        <v>2020</v>
+        <v>2013</v>
       </c>
       <c r="E17" s="1">
-        <v>7.2139999999999996E-2</v>
+        <v>5.79E-2</v>
       </c>
       <c r="F17" s="1">
-        <v>8.6360000000000006E-2</v>
+        <v>5.5629999999999999E-2</v>
       </c>
       <c r="G17" s="1">
-        <v>8.2460000000000006E-2</v>
+        <v>5.1639999999999998E-2</v>
       </c>
       <c r="H17" s="1">
-        <v>5.8470000000000001E-2</v>
+        <v>5.2519999999999997E-2</v>
       </c>
       <c r="I17" s="1">
-        <v>6.5250000000000002E-2</v>
+        <v>5.8930000000000003E-2</v>
       </c>
       <c r="J17" s="1">
-        <v>5.7099999999999998E-2</v>
+        <v>9.2700000000000005E-2</v>
       </c>
       <c r="K17" s="1">
-        <v>8.0140000000000003E-2</v>
+        <v>9.2100000000000001E-2</v>
       </c>
       <c r="L17" s="1">
-        <v>7.0860000000000006E-2</v>
+        <v>8.1600000000000006E-2</v>
       </c>
       <c r="M17" s="1">
-        <v>5.8900000000000001E-2</v>
+        <v>7.4899999999999994E-2</v>
       </c>
       <c r="N17" s="1">
-        <v>5.8779999999999999E-2</v>
+        <v>7.46E-2</v>
       </c>
       <c r="O17" s="1">
-        <v>0.1333</v>
+        <v>0.14929999999999999</v>
       </c>
       <c r="P17" s="1">
-        <v>7.9000000000000001E-2</v>
+        <v>7.886E-2</v>
       </c>
       <c r="Q17" s="1">
-        <v>6.1650000000000003E-2</v>
+        <v>5.466E-2</v>
       </c>
       <c r="R17" s="1">
-        <v>3.5639999999999998E-2</v>
+        <v>2.4639999999999999E-2</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>28656000</v>
+        <v>75633000</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="1">
-        <v>2013</v>
+        <v>2023</v>
       </c>
       <c r="E18" s="1">
-        <v>5.7070000000000003E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F18" s="1">
-        <v>5.0479999999999997E-2</v>
+        <v>7.5740000000000002E-2</v>
       </c>
       <c r="G18" s="1">
-        <v>4.19E-2</v>
+        <v>7.3550000000000004E-2</v>
       </c>
       <c r="H18" s="1">
-        <v>3.9669999999999997E-2</v>
+        <v>5.6270000000000001E-2</v>
       </c>
       <c r="I18" s="1">
-        <v>4.7359999999999999E-2</v>
+        <v>4.5870000000000001E-2</v>
       </c>
       <c r="J18" s="1">
-        <v>8.0699999999999994E-2</v>
+        <v>4.0370000000000003E-2</v>
       </c>
       <c r="K18" s="1">
-        <v>7.6600000000000001E-2</v>
+        <v>6.3350000000000004E-2</v>
       </c>
       <c r="L18" s="1">
-        <v>7.1999999999999995E-2</v>
+        <v>8.2400000000000001E-2</v>
       </c>
       <c r="M18" s="1">
-        <v>6.2230000000000001E-2</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="N18" s="1">
-        <v>7.8600000000000003E-2</v>
+        <v>7.7499999999999999E-2</v>
       </c>
       <c r="O18" s="1">
-        <v>0.18140000000000001</v>
+        <v>0.11285000000000001</v>
       </c>
       <c r="P18" s="1">
-        <v>9.4600000000000004E-2</v>
+        <v>6.2560000000000004E-2</v>
       </c>
       <c r="Q18" s="1">
-        <v>8.0699999999999994E-2</v>
+        <v>9.1399999999999995E-2</v>
       </c>
       <c r="R18" s="1">
-        <v>3.6799999999999999E-2</v>
+        <v>8.5199999999999998E-2</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>28656000</v>
+        <v>75633000</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="1">
-        <v>2013</v>
+        <v>2023</v>
       </c>
       <c r="E19" s="1">
-        <v>6.2260000000000003E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="F19" s="1">
-        <v>5.3530000000000001E-2</v>
+        <v>9.3799999999999994E-2</v>
       </c>
       <c r="G19" s="1">
-        <v>4.8739999999999999E-2</v>
+        <v>9.1800000000000007E-2</v>
       </c>
       <c r="H19" s="1">
-        <v>4.4159999999999998E-2</v>
+        <v>6.0299999999999999E-2</v>
       </c>
       <c r="I19" s="1">
-        <v>6.4449999999999993E-2</v>
+        <v>2.7019999999999999E-2</v>
       </c>
       <c r="J19" s="1">
-        <v>0.1017</v>
+        <v>3.8100000000000002E-2</v>
       </c>
       <c r="K19" s="1">
-        <v>8.6099999999999996E-2</v>
+        <v>8.1799999999999998E-2</v>
       </c>
       <c r="L19" s="1">
-        <v>7.5259999999999994E-2</v>
+        <v>9.0639999999999998E-2</v>
       </c>
       <c r="M19" s="1">
-        <v>6.4399999999999999E-2</v>
+        <v>7.4899999999999994E-2</v>
       </c>
       <c r="N19" s="1">
+        <v>7.3700000000000002E-2</v>
+      </c>
+      <c r="O19" s="1">
+        <v>0.1051</v>
+      </c>
+      <c r="P19" s="1">
+        <v>5.6730000000000003E-2</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="R19" s="1">
         <v>6.7599999999999993E-2</v>
-      </c>
-      <c r="O19" s="1">
-        <v>0.1588</v>
-      </c>
-      <c r="P19" s="1">
-        <v>7.9200000000000007E-2</v>
-      </c>
-      <c r="Q19" s="1">
-        <v>6.4299999999999996E-2</v>
-      </c>
-      <c r="R19" s="1">
-        <v>2.945E-2</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>98701000</v>
+        <v>28656000</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="1">
-        <v>2019</v>
+        <v>2013</v>
       </c>
       <c r="E20" s="1">
-        <v>8.3199999999999996E-2</v>
+        <v>5.7070000000000003E-2</v>
       </c>
       <c r="F20" s="1">
-        <v>8.5199999999999998E-2</v>
+        <v>5.0479999999999997E-2</v>
       </c>
       <c r="G20" s="1">
-        <v>6.7500000000000004E-2</v>
+        <v>4.19E-2</v>
       </c>
       <c r="H20" s="1">
-        <v>6.7900000000000002E-2</v>
+        <v>3.9669999999999997E-2</v>
       </c>
       <c r="I20" s="1">
-        <v>6.5729999999999997E-2</v>
+        <v>4.7359999999999999E-2</v>
       </c>
       <c r="J20" s="1">
-        <v>0.11176</v>
+        <v>8.0699999999999994E-2</v>
       </c>
       <c r="K20" s="1">
-        <v>0.1137</v>
+        <v>7.6600000000000001E-2</v>
       </c>
       <c r="L20" s="1">
-        <v>8.5999999999999993E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="M20" s="1">
-        <v>6.9000000000000006E-2</v>
+        <v>6.2230000000000001E-2</v>
       </c>
       <c r="N20" s="1">
-        <v>5.7979999999999997E-2</v>
+        <v>7.8600000000000003E-2</v>
       </c>
       <c r="O20" s="1">
-        <v>8.5099999999999995E-2</v>
+        <v>0.18140000000000001</v>
       </c>
       <c r="P20" s="1">
-        <v>4.5870000000000001E-2</v>
+        <v>9.4600000000000004E-2</v>
       </c>
       <c r="Q20" s="1">
-        <v>3.5369999999999999E-2</v>
+        <v>8.0699999999999994E-2</v>
       </c>
       <c r="R20" s="1">
-        <v>2.5729999999999999E-2</v>
+        <v>3.6799999999999999E-2</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>98701000</v>
+        <v>28656000</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="1">
-        <v>2019</v>
+        <v>2013</v>
       </c>
       <c r="E21" s="1">
-        <v>7.2499999999999995E-2</v>
+        <v>6.2260000000000003E-2</v>
       </c>
       <c r="F21" s="1">
-        <v>7.3359999999999995E-2</v>
+        <v>5.3530000000000001E-2</v>
       </c>
       <c r="G21" s="1">
-        <v>5.8799999999999998E-2</v>
+        <v>4.8739999999999999E-2</v>
       </c>
       <c r="H21" s="1">
-        <v>5.9900000000000002E-2</v>
+        <v>4.4159999999999998E-2</v>
       </c>
       <c r="I21" s="1">
-        <v>6.8540000000000004E-2</v>
+        <v>6.4449999999999993E-2</v>
       </c>
       <c r="J21" s="1">
-        <v>0.1115</v>
+        <v>0.1017</v>
       </c>
       <c r="K21" s="1">
-        <v>0.10376000000000001</v>
+        <v>8.6099999999999996E-2</v>
       </c>
       <c r="L21" s="1">
-        <v>0.08</v>
+        <v>7.5259999999999994E-2</v>
       </c>
       <c r="M21" s="1">
-        <v>6.7799999999999999E-2</v>
+        <v>6.4399999999999999E-2</v>
       </c>
       <c r="N21" s="1">
-        <v>5.9569999999999998E-2</v>
+        <v>6.7599999999999993E-2</v>
       </c>
       <c r="O21" s="1">
-        <v>9.8699999999999996E-2</v>
+        <v>0.1588</v>
       </c>
       <c r="P21" s="1">
-        <v>5.6550000000000003E-2</v>
+        <v>7.9200000000000007E-2</v>
       </c>
       <c r="Q21" s="1">
-        <v>4.8340000000000001E-2</v>
+        <v>6.4299999999999996E-2</v>
       </c>
       <c r="R21" s="1">
-        <v>4.0620000000000003E-2</v>
+        <v>2.945E-2</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>1630000</v>
+        <v>98701000</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="1">
-        <v>2023</v>
+        <v>2019</v>
       </c>
       <c r="E22" s="1">
-        <v>4.2720000000000001E-2</v>
+        <v>8.3199999999999996E-2</v>
       </c>
       <c r="F22" s="1">
-        <v>6.8849999999999995E-2</v>
+        <v>8.5199999999999998E-2</v>
       </c>
       <c r="G22" s="1">
-        <v>7.22E-2</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="H22" s="1">
-        <v>6.3899999999999998E-2</v>
+        <v>6.7900000000000002E-2</v>
       </c>
       <c r="I22" s="1">
-        <v>4.1750000000000002E-2</v>
+        <v>6.5729999999999997E-2</v>
       </c>
       <c r="J22" s="1">
-        <v>3.424E-2</v>
+        <v>0.11176</v>
       </c>
       <c r="K22" s="1">
-        <v>4.9770000000000002E-2</v>
+        <v>0.1137</v>
       </c>
       <c r="L22" s="1">
-        <v>8.0699999999999994E-2</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="M22" s="1">
-        <v>8.2150000000000001E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="N22" s="1">
-        <v>7.5800000000000006E-2</v>
+        <v>5.7979999999999997E-2</v>
       </c>
       <c r="O22" s="1">
-        <v>0.12085</v>
+        <v>8.5099999999999995E-2</v>
       </c>
       <c r="P22" s="1">
-        <v>6.726E-2</v>
+        <v>4.5870000000000001E-2</v>
       </c>
       <c r="Q22" s="1">
-        <v>0.1027</v>
+        <v>3.5369999999999999E-2</v>
       </c>
       <c r="R22" s="1">
-        <v>9.7100000000000006E-2</v>
+        <v>2.5729999999999999E-2</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>1630000</v>
+        <v>98701000</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D23" s="1">
-        <v>2023</v>
+        <v>2019</v>
       </c>
       <c r="E23" s="1">
-        <v>0.05</v>
+        <v>7.2499999999999995E-2</v>
       </c>
       <c r="F23" s="1">
-        <v>7.5700000000000003E-2</v>
+        <v>7.3359999999999995E-2</v>
       </c>
       <c r="G23" s="1">
-        <v>8.2799999999999999E-2</v>
+        <v>5.8799999999999998E-2</v>
       </c>
       <c r="H23" s="1">
-        <v>7.6300000000000007E-2</v>
+        <v>5.9900000000000002E-2</v>
       </c>
       <c r="I23" s="1">
-        <v>5.6149999999999999E-2</v>
+        <v>6.8540000000000004E-2</v>
       </c>
       <c r="J23" s="1">
-        <v>4.5260000000000002E-2</v>
+        <v>0.1115</v>
       </c>
       <c r="K23" s="1">
-        <v>5.8069999999999997E-2</v>
+        <v>0.10376000000000001</v>
       </c>
       <c r="L23" s="1">
-        <v>7.6999999999999999E-2</v>
+        <v>0.08</v>
       </c>
       <c r="M23" s="1">
-        <v>7.8899999999999998E-2</v>
+        <v>6.7799999999999999E-2</v>
       </c>
       <c r="N23" s="1">
-        <v>7.4800000000000005E-2</v>
+        <v>5.9569999999999998E-2</v>
       </c>
       <c r="O23" s="1">
-        <v>0.1106</v>
+        <v>9.8699999999999996E-2</v>
       </c>
       <c r="P23" s="1">
-        <v>6.2469999999999998E-2</v>
+        <v>5.6550000000000003E-2</v>
       </c>
       <c r="Q23" s="1">
-        <v>8.4199999999999997E-2</v>
+        <v>4.8340000000000001E-2</v>
       </c>
       <c r="R23" s="1">
-        <v>6.7699999999999996E-2</v>
+        <v>4.0620000000000003E-2</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -1888,10 +1888,10 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>33618000</v>
+        <v>80631000</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>18</v>
@@ -1900,54 +1900,54 @@
         <v>2020</v>
       </c>
       <c r="E26" s="1">
-        <v>4.514E-2</v>
+        <v>5.713E-2</v>
       </c>
       <c r="F26" s="1">
-        <v>6.9339999999999999E-2</v>
+        <v>6.6350000000000006E-2</v>
       </c>
       <c r="G26" s="1">
-        <v>5.6640000000000003E-2</v>
+        <v>6.54E-2</v>
       </c>
       <c r="H26" s="1">
-        <v>3.7350000000000001E-2</v>
+        <v>4.7969999999999999E-2</v>
       </c>
       <c r="I26" s="1">
-        <v>4.5319999999999999E-2</v>
+        <v>4.8160000000000001E-2</v>
       </c>
       <c r="J26" s="1">
-        <v>2.5250000000000002E-2</v>
+        <v>4.5749999999999999E-2</v>
       </c>
       <c r="K26" s="1">
-        <v>5.8169999999999999E-2</v>
+        <v>7.306E-2</v>
       </c>
       <c r="L26" s="1">
-        <v>6.7900000000000002E-2</v>
+        <v>7.0499999999999993E-2</v>
       </c>
       <c r="M26" s="1">
-        <v>6.3E-2</v>
+        <v>6.5699999999999995E-2</v>
       </c>
       <c r="N26" s="1">
-        <v>6.3839999999999994E-2</v>
+        <v>6.1429999999999998E-2</v>
       </c>
       <c r="O26" s="1">
-        <v>0.15229999999999999</v>
+        <v>0.14660000000000001</v>
       </c>
       <c r="P26" s="1">
-        <v>0.10034</v>
+        <v>9.0639999999999998E-2</v>
       </c>
       <c r="Q26" s="1">
-        <v>0.12164</v>
+        <v>8.7499999999999994E-2</v>
       </c>
       <c r="R26" s="1">
-        <v>9.3799999999999994E-2</v>
+        <v>7.3700000000000002E-2</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>33618000</v>
+        <v>80631000</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>19</v>
@@ -1956,382 +1956,382 @@
         <v>2020</v>
       </c>
       <c r="E27" s="1">
-        <v>5.1479999999999998E-2</v>
+        <v>6.1899999999999997E-2</v>
       </c>
       <c r="F27" s="1">
-        <v>7.7499999999999999E-2</v>
+        <v>7.1800000000000003E-2</v>
       </c>
       <c r="G27" s="1">
-        <v>5.9900000000000002E-2</v>
+        <v>6.9099999999999995E-2</v>
       </c>
       <c r="H27" s="1">
-        <v>4.0340000000000001E-2</v>
+        <v>5.1240000000000001E-2</v>
       </c>
       <c r="I27" s="1">
-        <v>4.2880000000000001E-2</v>
+        <v>4.446E-2</v>
       </c>
       <c r="J27" s="1">
-        <v>5.0840000000000003E-2</v>
+        <v>8.0439999999999998E-2</v>
       </c>
       <c r="K27" s="1">
-        <v>8.5750000000000007E-2</v>
+        <v>9.3899999999999997E-2</v>
       </c>
       <c r="L27" s="1">
-        <v>8.4000000000000005E-2</v>
+        <v>7.5130000000000002E-2</v>
       </c>
       <c r="M27" s="1">
-        <v>6.9339999999999999E-2</v>
+        <v>6.3600000000000004E-2</v>
       </c>
       <c r="N27" s="1">
-        <v>6.2899999999999998E-2</v>
+        <v>6.1039999999999997E-2</v>
       </c>
       <c r="O27" s="1">
-        <v>0.1323</v>
+        <v>0.1278</v>
       </c>
       <c r="P27" s="1">
-        <v>8.48E-2</v>
+        <v>7.6969999999999997E-2</v>
       </c>
       <c r="Q27" s="1">
-        <v>8.9399999999999993E-2</v>
+        <v>7.2900000000000006E-2</v>
       </c>
       <c r="R27" s="1">
-        <v>6.8540000000000004E-2</v>
+        <v>4.9840000000000002E-2</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>38701000</v>
+        <v>80601000</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D28" s="1">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="E28" s="1">
-        <v>4.2900000000000001E-2</v>
+        <v>7.2270000000000001E-2</v>
       </c>
       <c r="F28" s="1">
-        <v>5.9499999999999997E-2</v>
+        <v>8.7160000000000001E-2</v>
       </c>
       <c r="G28" s="1">
-        <v>5.475E-2</v>
+        <v>8.0140000000000003E-2</v>
       </c>
       <c r="H28" s="1">
-        <v>4.8550000000000003E-2</v>
+        <v>5.5300000000000002E-2</v>
       </c>
       <c r="I28" s="1">
-        <v>4.48E-2</v>
+        <v>5.79E-2</v>
       </c>
       <c r="J28" s="1">
-        <v>4.9930000000000002E-2</v>
+        <v>4.1930000000000002E-2</v>
       </c>
       <c r="K28" s="1">
-        <v>7.6899999999999996E-2</v>
+        <v>6.9599999999999995E-2</v>
       </c>
       <c r="L28" s="1">
-        <v>9.2039999999999997E-2</v>
+        <v>6.2469999999999998E-2</v>
       </c>
       <c r="M28" s="1">
-        <v>8.1799999999999998E-2</v>
+        <v>6.2560000000000004E-2</v>
       </c>
       <c r="N28" s="1">
-        <v>7.6100000000000001E-2</v>
+        <v>5.91E-2</v>
       </c>
       <c r="O28" s="1">
-        <v>0.12427000000000001</v>
+        <v>0.14610000000000001</v>
       </c>
       <c r="P28" s="1">
-        <v>7.0400000000000004E-2</v>
+        <v>8.5139999999999993E-2</v>
       </c>
       <c r="Q28" s="1">
-        <v>9.0700000000000003E-2</v>
+        <v>7.1900000000000006E-2</v>
       </c>
       <c r="R28" s="1">
-        <v>8.7340000000000001E-2</v>
+        <v>4.8500000000000001E-2</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>38701000</v>
+        <v>80601000</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="1">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="E29" s="1">
-        <v>5.4960000000000002E-2</v>
+        <v>7.2139999999999996E-2</v>
       </c>
       <c r="F29" s="1">
-        <v>7.3400000000000007E-2</v>
+        <v>8.6360000000000006E-2</v>
       </c>
       <c r="G29" s="1">
-        <v>6.744E-2</v>
+        <v>8.2460000000000006E-2</v>
       </c>
       <c r="H29" s="1">
-        <v>6.1460000000000001E-2</v>
+        <v>5.8470000000000001E-2</v>
       </c>
       <c r="I29" s="1">
-        <v>4.82E-2</v>
+        <v>6.5250000000000002E-2</v>
       </c>
       <c r="J29" s="1">
-        <v>5.2060000000000002E-2</v>
+        <v>5.7099999999999998E-2</v>
       </c>
       <c r="K29" s="1">
-        <v>7.9200000000000007E-2</v>
+        <v>8.0140000000000003E-2</v>
       </c>
       <c r="L29" s="1">
-        <v>9.7000000000000003E-2</v>
+        <v>7.0860000000000006E-2</v>
       </c>
       <c r="M29" s="1">
-        <v>8.4839999999999999E-2</v>
+        <v>5.8900000000000001E-2</v>
       </c>
       <c r="N29" s="1">
-        <v>7.6100000000000001E-2</v>
+        <v>5.8779999999999999E-2</v>
       </c>
       <c r="O29" s="1">
-        <v>0.11269999999999999</v>
+        <v>0.1333</v>
       </c>
       <c r="P29" s="1">
-        <v>6.1600000000000002E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="Q29" s="1">
-        <v>7.1529999999999996E-2</v>
+        <v>6.1650000000000003E-2</v>
       </c>
       <c r="R29" s="1">
-        <v>5.9630000000000002E-2</v>
+        <v>3.5639999999999998E-2</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>20627000</v>
+        <v>38701000</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D30" s="1">
-        <v>2012</v>
+        <v>2023</v>
       </c>
       <c r="E30" s="1">
-        <v>5.9569999999999998E-2</v>
+        <v>4.2900000000000001E-2</v>
       </c>
       <c r="F30" s="1">
-        <v>5.3039999999999997E-2</v>
+        <v>5.9499999999999997E-2</v>
       </c>
       <c r="G30" s="1">
-        <v>5.57E-2</v>
+        <v>5.475E-2</v>
       </c>
       <c r="H30" s="1">
-        <v>5.1450000000000003E-2</v>
+        <v>4.8550000000000003E-2</v>
       </c>
       <c r="I30" s="1">
-        <v>6.5369999999999998E-2</v>
+        <v>4.48E-2</v>
       </c>
       <c r="J30" s="1">
-        <v>7.7899999999999997E-2</v>
+        <v>4.9930000000000002E-2</v>
       </c>
       <c r="K30" s="1">
         <v>7.6899999999999996E-2</v>
       </c>
       <c r="L30" s="1">
-        <v>7.6999999999999999E-2</v>
+        <v>9.2039999999999997E-2</v>
       </c>
       <c r="M30" s="1">
-        <v>7.4999999999999997E-2</v>
+        <v>8.1799999999999998E-2</v>
       </c>
       <c r="N30" s="1">
-        <v>8.6099999999999996E-2</v>
+        <v>7.6100000000000001E-2</v>
       </c>
       <c r="O30" s="1">
-        <v>0.10284</v>
+        <v>0.12427000000000001</v>
       </c>
       <c r="P30" s="1">
-        <v>8.9099999999999999E-2</v>
+        <v>7.0400000000000004E-2</v>
       </c>
       <c r="Q30" s="1">
-        <v>8.5599999999999996E-2</v>
+        <v>9.0700000000000003E-2</v>
       </c>
       <c r="R30" s="1">
-        <v>4.4400000000000002E-2</v>
+        <v>8.7340000000000001E-2</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>20627000</v>
+        <v>38701000</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D31" s="1">
-        <v>2012</v>
+        <v>2023</v>
       </c>
       <c r="E31" s="1">
-        <v>6.1280000000000001E-2</v>
+        <v>5.4960000000000002E-2</v>
       </c>
       <c r="F31" s="1">
-        <v>5.9360000000000003E-2</v>
+        <v>7.3400000000000007E-2</v>
       </c>
       <c r="G31" s="1">
-        <v>6.4899999999999999E-2</v>
+        <v>6.744E-2</v>
       </c>
       <c r="H31" s="1">
-        <v>6.3600000000000004E-2</v>
+        <v>6.1460000000000001E-2</v>
       </c>
       <c r="I31" s="1">
-        <v>7.1400000000000005E-2</v>
+        <v>4.82E-2</v>
       </c>
       <c r="J31" s="1">
-        <v>8.8599999999999998E-2</v>
+        <v>5.2060000000000002E-2</v>
       </c>
       <c r="K31" s="1">
-        <v>7.6700000000000004E-2</v>
+        <v>7.9200000000000007E-2</v>
       </c>
       <c r="L31" s="1">
-        <v>7.6300000000000007E-2</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="M31" s="1">
-        <v>7.4300000000000005E-2</v>
+        <v>8.4839999999999999E-2</v>
       </c>
       <c r="N31" s="1">
-        <v>8.6300000000000002E-2</v>
+        <v>7.6100000000000001E-2</v>
       </c>
       <c r="O31" s="1">
-        <v>0.10297000000000001</v>
+        <v>0.11269999999999999</v>
       </c>
       <c r="P31" s="1">
-        <v>8.0699999999999994E-2</v>
+        <v>6.1600000000000002E-2</v>
       </c>
       <c r="Q31" s="1">
-        <v>6.6650000000000001E-2</v>
+        <v>7.1529999999999996E-2</v>
       </c>
       <c r="R31" s="1">
-        <v>2.6980000000000001E-2</v>
+        <v>5.9630000000000002E-2</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>11710000</v>
+        <v>20627000</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D32" s="1">
-        <v>2019</v>
+        <v>2012</v>
       </c>
       <c r="E32" s="1">
-        <v>5.8799999999999998E-2</v>
+        <v>5.9569999999999998E-2</v>
       </c>
       <c r="F32" s="1">
-        <v>6.7799999999999999E-2</v>
+        <v>5.3039999999999997E-2</v>
       </c>
       <c r="G32" s="1">
-        <v>6.0400000000000002E-2</v>
+        <v>5.57E-2</v>
       </c>
       <c r="H32" s="1">
-        <v>4.6899999999999997E-2</v>
+        <v>5.1450000000000003E-2</v>
       </c>
       <c r="I32" s="1">
-        <v>3.168E-2</v>
+        <v>6.5369999999999998E-2</v>
       </c>
       <c r="J32" s="1">
-        <v>4.7940000000000003E-2</v>
+        <v>7.7899999999999997E-2</v>
       </c>
       <c r="K32" s="1">
-        <v>7.7149999999999996E-2</v>
+        <v>7.6899999999999996E-2</v>
       </c>
       <c r="L32" s="1">
-        <v>8.6550000000000002E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="M32" s="1">
-        <v>8.0259999999999998E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="N32" s="1">
-        <v>6.3049999999999995E-2</v>
+        <v>8.6099999999999996E-2</v>
       </c>
       <c r="O32" s="1">
-        <v>0.12759999999999999</v>
+        <v>0.10284</v>
       </c>
       <c r="P32" s="1">
-        <v>8.0399999999999999E-2</v>
+        <v>8.9099999999999999E-2</v>
       </c>
       <c r="Q32" s="1">
-        <v>9.3700000000000006E-2</v>
+        <v>8.5599999999999996E-2</v>
       </c>
       <c r="R32" s="1">
-        <v>7.7899999999999997E-2</v>
+        <v>4.4400000000000002E-2</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>11710000</v>
+        <v>20627000</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D33" s="1">
-        <v>2019</v>
+        <v>2012</v>
       </c>
       <c r="E33" s="1">
-        <v>7.0430000000000006E-2</v>
+        <v>6.1280000000000001E-2</v>
       </c>
       <c r="F33" s="1">
-        <v>8.2150000000000001E-2</v>
+        <v>5.9360000000000003E-2</v>
       </c>
       <c r="G33" s="1">
-        <v>6.9760000000000003E-2</v>
+        <v>6.4899999999999999E-2</v>
       </c>
       <c r="H33" s="1">
-        <v>5.4100000000000002E-2</v>
+        <v>6.3600000000000004E-2</v>
       </c>
       <c r="I33" s="1">
-        <v>2.7189999999999999E-2</v>
+        <v>7.1400000000000005E-2</v>
       </c>
       <c r="J33" s="1">
-        <v>4.8550000000000003E-2</v>
+        <v>8.8599999999999998E-2</v>
       </c>
       <c r="K33" s="1">
-        <v>8.7999999999999995E-2</v>
+        <v>7.6700000000000004E-2</v>
       </c>
       <c r="L33" s="1">
-        <v>0.10009999999999999</v>
+        <v>7.6300000000000007E-2</v>
       </c>
       <c r="M33" s="1">
-        <v>9.4539999999999999E-2</v>
+        <v>7.4300000000000005E-2</v>
       </c>
       <c r="N33" s="1">
-        <v>6.83E-2</v>
+        <v>8.6300000000000002E-2</v>
       </c>
       <c r="O33" s="1">
-        <v>0.11115</v>
+        <v>0.10297000000000001</v>
       </c>
       <c r="P33" s="1">
-        <v>6.7500000000000004E-2</v>
+        <v>8.0699999999999994E-2</v>
       </c>
       <c r="Q33" s="1">
-        <v>6.6500000000000004E-2</v>
+        <v>6.6650000000000001E-2</v>
       </c>
       <c r="R33" s="1">
-        <v>5.1670000000000001E-2</v>
+        <v>2.6980000000000001E-2</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>